<commit_message>
Updated test cases, assumptions, added bug report with bugs i assumed
</commit_message>
<xml_diff>
--- a/Bug Report.xlsx
+++ b/Bug Report.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\QualityHub\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA1D4418-B951-4DCA-BDCA-06801D8FDDFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,9 +24,125 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="37">
+  <si>
+    <t>Bug ID</t>
+  </si>
+  <si>
+    <t>Bug Title</t>
+  </si>
+  <si>
+    <t>Frontal Area allows string value</t>
+  </si>
+  <si>
+    <t>Bug Description</t>
+  </si>
+  <si>
+    <t>When WLTP relevancy value is Yes for WLTP, user need to input "Frontal Area" with integer value. Frontal Area field is string data type.</t>
+  </si>
+  <si>
+    <t>1. Login in to the application</t>
+  </si>
+  <si>
+    <t>2. Go to WTLP data from left navigation menu or click WTLP data on dashboard</t>
+  </si>
+  <si>
+    <t>3. Add or Edit WTLP data by clicking on 'Create WLTP Data' button or by clicking on existing WTLP data from list respectively</t>
+  </si>
+  <si>
+    <t>4. Enter all required field values</t>
+  </si>
+  <si>
+    <t>5. Select Yes for WLTP relevancy value</t>
+  </si>
+  <si>
+    <t>6. User should be able to enter "Frontal Area" value</t>
+  </si>
+  <si>
+    <t>7. Enter "STRONG" (or any String value) into the "Frontal Area" field</t>
+  </si>
+  <si>
+    <t>8. Save WTLP data</t>
+  </si>
+  <si>
+    <t>Expected Result</t>
+  </si>
+  <si>
+    <t>The "Frontal Area" should be stored as an integer</t>
+  </si>
+  <si>
+    <t>Actual Result</t>
+  </si>
+  <si>
+    <t>User was able to save WTLP data with Frontal Area with string value</t>
+  </si>
+  <si>
+    <t>Severity</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>Environment</t>
+  </si>
+  <si>
+    <t>Staging</t>
+  </si>
+  <si>
+    <t>Reported by</t>
+  </si>
+  <si>
+    <t>Silu Pandit</t>
+  </si>
+  <si>
+    <t>Reported on</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>New</t>
+  </si>
+  <si>
+    <t>Assigned To</t>
+  </si>
+  <si>
+    <t>Dev Lead</t>
+  </si>
+  <si>
+    <t>MasterCode exceeded 3 characters limit.</t>
+  </si>
+  <si>
+    <t>When creating new product MasterCode field should only have 3 characters.</t>
+  </si>
+  <si>
+    <t>2. Go to Product from left navigation menu or click Product on dashboard</t>
+  </si>
+  <si>
+    <t>3. Add or Edit Product by clicking on 'Create Product' button or by clicking on existing product from list respectively</t>
+  </si>
+  <si>
+    <t>5. Enter MasterCode with more than 3 characters</t>
+  </si>
+  <si>
+    <t>MasterCode field should not exceed 3 characters limit.</t>
+  </si>
+  <si>
+    <t>Steps to replicate</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -28,16 +150,45 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3A3A3A"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3A3A3A"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -45,12 +196,53 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,13 +522,349 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="30.1328125" customWidth="1"/>
+    <col min="2" max="2" width="108.3984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A3" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A4" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A5" s="8"/>
+      <c r="B5" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A6" s="8"/>
+      <c r="B6" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A7" s="8"/>
+      <c r="B7" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A8" s="8"/>
+      <c r="B8" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A9" s="8"/>
+      <c r="B9" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A10" s="8"/>
+      <c r="B10" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A11" s="8"/>
+      <c r="B11" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A12" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A13" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A14" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A15" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A16" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A17" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A18" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" s="9">
+        <v>45131</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A19" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A20" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A23" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23" s="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A24" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A25" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A26" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A27" s="8"/>
+      <c r="B27" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A28" s="8"/>
+      <c r="B28" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A29" s="8"/>
+      <c r="B29" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A30" s="8"/>
+      <c r="B30" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A31" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A32" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A33" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A34" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A35" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A36" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A37" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B37" s="9">
+        <v>45131</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A38" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A39" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A62" s="1"/>
+      <c r="B62" s="2"/>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A63" s="1"/>
+      <c r="B63" s="2"/>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A64" s="1"/>
+      <c r="B64" s="2"/>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A65" s="1"/>
+      <c r="B65" s="2"/>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A66" s="3"/>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A67" s="3"/>
+      <c r="B67" s="2"/>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A68" s="3"/>
+      <c r="B68" s="2"/>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A69" s="3"/>
+      <c r="B69" s="2"/>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A70" s="3"/>
+      <c r="B70" s="2"/>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A71" s="3"/>
+      <c r="B71" s="2"/>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A72" s="3"/>
+      <c r="B72" s="4"/>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A73" s="3"/>
+      <c r="B73" s="2"/>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A74" s="3"/>
+      <c r="B74" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A4:A11"/>
+    <mergeCell ref="A26:A30"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>